<commit_message>
docs: actualización preliminar de 1FN
</commit_message>
<xml_diff>
--- a/docs/Base de datos/Diagramas/Formas Normales/2FN.xlsx
+++ b/docs/Base de datos/Diagramas/Formas Normales/2FN.xlsx
@@ -11,18 +11,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Instituciones</t>
   </si>
   <si>
+    <t>Material académico</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>ID_Institución</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>ID_Material</t>
+  </si>
+  <si>
+    <t>Materia</t>
+  </si>
+  <si>
+    <t>ID_Nota</t>
+  </si>
+  <si>
+    <t>Alumno</t>
+  </si>
+  <si>
+    <t>Examen</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>San Pablo</t>
+  </si>
+  <si>
+    <t>BD7.pdf</t>
+  </si>
+  <si>
+    <t>Carreras</t>
+  </si>
+  <si>
+    <t>Materias</t>
+  </si>
+  <si>
+    <t>ID_Carrera</t>
+  </si>
+  <si>
+    <t>Institución</t>
+  </si>
+  <si>
+    <t>ID_Materia</t>
+  </si>
+  <si>
+    <t>Sistemas</t>
+  </si>
+  <si>
+    <t>Base de datos</t>
+  </si>
+  <si>
+    <t>Cursos</t>
+  </si>
+  <si>
     <t>Profesores</t>
   </si>
   <si>
-    <t>ID_Institución</t>
-  </si>
-  <si>
-    <t>Nombre</t>
+    <t>ID_Curso</t>
+  </si>
+  <si>
+    <t>División</t>
+  </si>
+  <si>
+    <t>Carrera</t>
   </si>
   <si>
     <t>ID_Profesor</t>
@@ -31,7 +94,7 @@
     <t>Apellido</t>
   </si>
   <si>
-    <t>San Pablo</t>
+    <t>a</t>
   </si>
   <si>
     <t>Rotilli</t>
@@ -40,16 +103,10 @@
     <t>Nicolás</t>
   </si>
   <si>
-    <t>Carreras</t>
-  </si>
-  <si>
     <t>Alumnos</t>
   </si>
   <si>
-    <t>ID_Carrera</t>
-  </si>
-  <si>
-    <t>Institución</t>
+    <t>Profesores-Materias</t>
   </si>
   <si>
     <t>ID_Alumno</t>
@@ -58,7 +115,10 @@
     <t>Curso</t>
   </si>
   <si>
-    <t>Sistemas</t>
+    <t>ID_P-M</t>
+  </si>
+  <si>
+    <t>Profesor</t>
   </si>
   <si>
     <t>Joaquín</t>
@@ -67,88 +127,28 @@
     <t>Borrás</t>
   </si>
   <si>
-    <t>Cursos</t>
-  </si>
-  <si>
     <t>Asistencias</t>
   </si>
   <si>
-    <t>ID_Curso</t>
-  </si>
-  <si>
-    <t>División</t>
-  </si>
-  <si>
-    <t>Carrera</t>
+    <t>Exámenes</t>
   </si>
   <si>
     <t>ID_Asistencia</t>
   </si>
   <si>
-    <t>Alumno</t>
-  </si>
-  <si>
-    <t>Materia-Profe.</t>
-  </si>
-  <si>
     <t>Presente</t>
   </si>
   <si>
+    <t>ID_Examen</t>
+  </si>
+  <si>
+    <t>Número</t>
+  </si>
+  <si>
     <t>Fecha</t>
   </si>
   <si>
-    <t>La asistencia puede ser por materia, profesor, media falta</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Fechas</t>
-  </si>
-  <si>
-    <t>Notas</t>
-  </si>
-  <si>
-    <t>ID_Fecha</t>
-  </si>
-  <si>
-    <t>Hábil</t>
-  </si>
-  <si>
-    <t>ID_Nota</t>
-  </si>
-  <si>
-    <t>Nota</t>
-  </si>
-  <si>
-    <t>Materias</t>
-  </si>
-  <si>
-    <t>Material académico</t>
-  </si>
-  <si>
-    <t>ID_Materia</t>
-  </si>
-  <si>
-    <t>ID_Material</t>
-  </si>
-  <si>
-    <t>Base de datos</t>
-  </si>
-  <si>
-    <t>BD7.pdf</t>
-  </si>
-  <si>
-    <t>Materias-Profesores</t>
-  </si>
-  <si>
-    <t>ID_MP</t>
-  </si>
-  <si>
-    <t>Materia</t>
-  </si>
-  <si>
-    <t>Profesor</t>
+    <t>Profe.-Materias</t>
   </si>
 </sst>
 </file>
@@ -171,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,20 +204,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEFEFEF"/>
-        <bgColor rgb="FFEFEFEF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF9CB9C"/>
         <bgColor rgb="FFF9CB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEAD1DC"/>
-        <bgColor rgb="FFEAD1DC"/>
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
   </fills>
@@ -241,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -266,19 +260,15 @@
     <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="7" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -506,169 +496,166 @@
       <c r="G4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="L4" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4"/>
       <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>5</v>
+      <c r="I5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>6</v>
+      <c r="B6" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="G6" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>8</v>
+      <c r="G6" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="L6" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="M6" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="N6" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="O6" s="7">
+        <v>10.0</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="G10" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="6">
-        <v>1.0</v>
+      <c r="B10" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="H13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="7" t="s">
+    </row>
+    <row r="14">
+      <c r="B14" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="C14" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="E14" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G14" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C14" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="I14" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="G14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="H14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="I14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="J14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="K14" s="6">
-        <v>1.0</v>
       </c>
     </row>
     <row r="16">
@@ -684,189 +671,165 @@
         <v>32</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>33</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="H17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="7" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="18">
-      <c r="B18" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C18" s="10">
+      <c r="B18" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G18" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="H18" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I18" s="7">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10"/>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10"/>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10"/>
+      <c r="B22" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="H22" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I22" s="11">
         <v>45525.0</v>
       </c>
-      <c r="D18" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="G18" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="H18" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="I18" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="J18" s="6">
+      <c r="J22" s="7">
         <v>10.0</v>
       </c>
-      <c r="K18" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="11"/>
-      <c r="B20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="11"/>
-      <c r="B21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="11"/>
-      <c r="B22" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="I22" s="13">
-        <v>1.0</v>
-      </c>
     </row>
     <row r="23">
-      <c r="A23" s="11"/>
+      <c r="A23" s="10"/>
     </row>
     <row r="24">
-      <c r="A24" s="11"/>
-      <c r="G24" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A24" s="10"/>
     </row>
     <row r="25">
-      <c r="A25" s="11"/>
-      <c r="G25" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="A25" s="10"/>
     </row>
     <row r="26">
-      <c r="A26" s="11"/>
-      <c r="G26" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="H26" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="I26" s="6">
-        <v>1.0</v>
-      </c>
+      <c r="A26" s="10"/>
     </row>
     <row r="27">
-      <c r="A27" s="11"/>
-      <c r="G27" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="H27" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="I27" s="6">
-        <v>2.0</v>
-      </c>
+      <c r="A27" s="10"/>
     </row>
     <row r="28">
-      <c r="A28" s="11"/>
+      <c r="A28" s="10"/>
     </row>
     <row r="29">
-      <c r="A29" s="11"/>
+      <c r="A29" s="10"/>
     </row>
     <row r="30">
-      <c r="A30" s="11"/>
+      <c r="A30" s="10"/>
     </row>
     <row r="31">
-      <c r="A31" s="11"/>
+      <c r="A31" s="10"/>
     </row>
     <row r="32">
-      <c r="A32" s="11"/>
+      <c r="A32" s="10"/>
     </row>
     <row r="33">
-      <c r="A33" s="11"/>
+      <c r="A33" s="10"/>
     </row>
     <row r="34">
-      <c r="A34" s="11"/>
+      <c r="A34" s="10"/>
     </row>
     <row r="35">
-      <c r="A35" s="11"/>
+      <c r="A35" s="10"/>
     </row>
     <row r="36">
-      <c r="A36" s="11"/>
+      <c r="A36" s="10"/>
     </row>
     <row r="37">
-      <c r="A37" s="11"/>
+      <c r="A37" s="10"/>
     </row>
     <row r="38">
-      <c r="A38" s="11"/>
+      <c r="A38" s="10"/>
     </row>
     <row r="39">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G12:I12"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>